<commit_message>
Update to only write 1 tmp img
</commit_message>
<xml_diff>
--- a/IPython/rdkit_hackaton/demo.xlsx
+++ b/IPython/rdkit_hackaton/demo.xlsx
@@ -3089,7 +3089,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="xlsx_tmp_img_1.png"/>
+        <xdr:cNvPr id="2" name="Picture 1" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3127,7 +3127,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2" descr="xlsx_tmp_img_2.png"/>
+        <xdr:cNvPr id="3" name="Picture 2" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3165,7 +3165,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3" descr="xlsx_tmp_img_3.png"/>
+        <xdr:cNvPr id="4" name="Picture 3" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3203,7 +3203,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4" descr="xlsx_tmp_img_4.png"/>
+        <xdr:cNvPr id="5" name="Picture 4" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3241,7 +3241,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5" descr="xlsx_tmp_img_5.png"/>
+        <xdr:cNvPr id="6" name="Picture 5" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3279,7 +3279,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6" descr="xlsx_tmp_img_6.png"/>
+        <xdr:cNvPr id="7" name="Picture 6" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3317,7 +3317,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 7" descr="xlsx_tmp_img_7.png"/>
+        <xdr:cNvPr id="8" name="Picture 7" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3355,7 +3355,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Picture 8" descr="xlsx_tmp_img_8.png"/>
+        <xdr:cNvPr id="9" name="Picture 8" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3393,7 +3393,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Picture 9" descr="xlsx_tmp_img_9.png"/>
+        <xdr:cNvPr id="10" name="Picture 9" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3431,7 +3431,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Picture 10" descr="xlsx_tmp_img_10.png"/>
+        <xdr:cNvPr id="11" name="Picture 10" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3469,7 +3469,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="Picture 11" descr="xlsx_tmp_img_11.png"/>
+        <xdr:cNvPr id="12" name="Picture 11" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3507,7 +3507,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="Picture 12" descr="xlsx_tmp_img_12.png"/>
+        <xdr:cNvPr id="13" name="Picture 12" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3545,7 +3545,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="14" name="Picture 13" descr="xlsx_tmp_img_13.png"/>
+        <xdr:cNvPr id="14" name="Picture 13" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3583,7 +3583,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="15" name="Picture 14" descr="xlsx_tmp_img_14.png"/>
+        <xdr:cNvPr id="15" name="Picture 14" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3621,7 +3621,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="16" name="Picture 15" descr="xlsx_tmp_img_15.png"/>
+        <xdr:cNvPr id="16" name="Picture 15" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3659,7 +3659,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="17" name="Picture 16" descr="xlsx_tmp_img_16.png"/>
+        <xdr:cNvPr id="17" name="Picture 16" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3697,7 +3697,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="18" name="Picture 17" descr="xlsx_tmp_img_17.png"/>
+        <xdr:cNvPr id="18" name="Picture 17" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3735,7 +3735,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="19" name="Picture 18" descr="xlsx_tmp_img_18.png"/>
+        <xdr:cNvPr id="19" name="Picture 18" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3773,7 +3773,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="20" name="Picture 19" descr="xlsx_tmp_img_19.png"/>
+        <xdr:cNvPr id="20" name="Picture 19" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3811,7 +3811,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="21" name="Picture 20" descr="xlsx_tmp_img_20.png"/>
+        <xdr:cNvPr id="21" name="Picture 20" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3849,7 +3849,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="22" name="Picture 21" descr="xlsx_tmp_img_21.png"/>
+        <xdr:cNvPr id="22" name="Picture 21" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3887,7 +3887,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="23" name="Picture 22" descr="xlsx_tmp_img_22.png"/>
+        <xdr:cNvPr id="23" name="Picture 22" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3925,7 +3925,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="24" name="Picture 23" descr="xlsx_tmp_img_23.png"/>
+        <xdr:cNvPr id="24" name="Picture 23" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3963,7 +3963,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="25" name="Picture 24" descr="xlsx_tmp_img_24.png"/>
+        <xdr:cNvPr id="25" name="Picture 24" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -4001,7 +4001,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="26" name="Picture 25" descr="xlsx_tmp_img_25.png"/>
+        <xdr:cNvPr id="26" name="Picture 25" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -4039,7 +4039,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="27" name="Picture 26" descr="xlsx_tmp_img_26.png"/>
+        <xdr:cNvPr id="27" name="Picture 26" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -4077,7 +4077,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="28" name="Picture 27" descr="xlsx_tmp_img_27.png"/>
+        <xdr:cNvPr id="28" name="Picture 27" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -4115,7 +4115,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="29" name="Picture 28" descr="xlsx_tmp_img_28.png"/>
+        <xdr:cNvPr id="29" name="Picture 28" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -4153,7 +4153,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="30" name="Picture 29" descr="xlsx_tmp_img_29.png"/>
+        <xdr:cNvPr id="30" name="Picture 29" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -4191,7 +4191,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="31" name="Picture 30" descr="xlsx_tmp_img_30.png"/>
+        <xdr:cNvPr id="31" name="Picture 30" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -4229,7 +4229,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="32" name="Picture 31" descr="xlsx_tmp_img_31.png"/>
+        <xdr:cNvPr id="32" name="Picture 31" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -4267,7 +4267,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="33" name="Picture 32" descr="xlsx_tmp_img_32.png"/>
+        <xdr:cNvPr id="33" name="Picture 32" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -4305,7 +4305,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="34" name="Picture 33" descr="xlsx_tmp_img_33.png"/>
+        <xdr:cNvPr id="34" name="Picture 33" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -4343,7 +4343,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="35" name="Picture 34" descr="xlsx_tmp_img_34.png"/>
+        <xdr:cNvPr id="35" name="Picture 34" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -4381,7 +4381,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="36" name="Picture 35" descr="xlsx_tmp_img_35.png"/>
+        <xdr:cNvPr id="36" name="Picture 35" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -4419,7 +4419,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="37" name="Picture 36" descr="xlsx_tmp_img_36.png"/>
+        <xdr:cNvPr id="37" name="Picture 36" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -4457,7 +4457,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="38" name="Picture 37" descr="xlsx_tmp_img_37.png"/>
+        <xdr:cNvPr id="38" name="Picture 37" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -4495,7 +4495,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="39" name="Picture 38" descr="xlsx_tmp_img_38.png"/>
+        <xdr:cNvPr id="39" name="Picture 38" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -4533,7 +4533,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="40" name="Picture 39" descr="xlsx_tmp_img_39.png"/>
+        <xdr:cNvPr id="40" name="Picture 39" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -4571,7 +4571,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="41" name="Picture 40" descr="xlsx_tmp_img_40.png"/>
+        <xdr:cNvPr id="41" name="Picture 40" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -4609,7 +4609,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="42" name="Picture 41" descr="xlsx_tmp_img_41.png"/>
+        <xdr:cNvPr id="42" name="Picture 41" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -4647,7 +4647,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="43" name="Picture 42" descr="xlsx_tmp_img_42.png"/>
+        <xdr:cNvPr id="43" name="Picture 42" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -4685,7 +4685,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="44" name="Picture 43" descr="xlsx_tmp_img_43.png"/>
+        <xdr:cNvPr id="44" name="Picture 43" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -4723,7 +4723,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="45" name="Picture 44" descr="xlsx_tmp_img_44.png"/>
+        <xdr:cNvPr id="45" name="Picture 44" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -4761,7 +4761,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="46" name="Picture 45" descr="xlsx_tmp_img_45.png"/>
+        <xdr:cNvPr id="46" name="Picture 45" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -4799,7 +4799,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="47" name="Picture 46" descr="xlsx_tmp_img_46.png"/>
+        <xdr:cNvPr id="47" name="Picture 46" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -4837,7 +4837,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="48" name="Picture 47" descr="xlsx_tmp_img_47.png"/>
+        <xdr:cNvPr id="48" name="Picture 47" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -4875,7 +4875,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="49" name="Picture 48" descr="xlsx_tmp_img_48.png"/>
+        <xdr:cNvPr id="49" name="Picture 48" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -4913,7 +4913,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="50" name="Picture 49" descr="xlsx_tmp_img_49.png"/>
+        <xdr:cNvPr id="50" name="Picture 49" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -4951,7 +4951,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="51" name="Picture 50" descr="xlsx_tmp_img_50.png"/>
+        <xdr:cNvPr id="51" name="Picture 50" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -4989,7 +4989,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="52" name="Picture 51" descr="xlsx_tmp_img_51.png"/>
+        <xdr:cNvPr id="52" name="Picture 51" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -5027,7 +5027,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="53" name="Picture 52" descr="xlsx_tmp_img_52.png"/>
+        <xdr:cNvPr id="53" name="Picture 52" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -5065,7 +5065,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="54" name="Picture 53" descr="xlsx_tmp_img_53.png"/>
+        <xdr:cNvPr id="54" name="Picture 53" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -5103,7 +5103,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="55" name="Picture 54" descr="xlsx_tmp_img_54.png"/>
+        <xdr:cNvPr id="55" name="Picture 54" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -5141,7 +5141,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="56" name="Picture 55" descr="xlsx_tmp_img_55.png"/>
+        <xdr:cNvPr id="56" name="Picture 55" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -5179,7 +5179,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="57" name="Picture 56" descr="xlsx_tmp_img_56.png"/>
+        <xdr:cNvPr id="57" name="Picture 56" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -5217,7 +5217,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="58" name="Picture 57" descr="xlsx_tmp_img_57.png"/>
+        <xdr:cNvPr id="58" name="Picture 57" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -5255,7 +5255,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="59" name="Picture 58" descr="xlsx_tmp_img_58.png"/>
+        <xdr:cNvPr id="59" name="Picture 58" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -5293,7 +5293,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="60" name="Picture 59" descr="xlsx_tmp_img_59.png"/>
+        <xdr:cNvPr id="60" name="Picture 59" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -5331,7 +5331,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="61" name="Picture 60" descr="xlsx_tmp_img_60.png"/>
+        <xdr:cNvPr id="61" name="Picture 60" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -5369,7 +5369,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="62" name="Picture 61" descr="xlsx_tmp_img_61.png"/>
+        <xdr:cNvPr id="62" name="Picture 61" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -5407,7 +5407,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="63" name="Picture 62" descr="xlsx_tmp_img_62.png"/>
+        <xdr:cNvPr id="63" name="Picture 62" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -5445,7 +5445,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="64" name="Picture 63" descr="xlsx_tmp_img_63.png"/>
+        <xdr:cNvPr id="64" name="Picture 63" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -5483,7 +5483,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="65" name="Picture 64" descr="xlsx_tmp_img_64.png"/>
+        <xdr:cNvPr id="65" name="Picture 64" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -5521,7 +5521,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="66" name="Picture 65" descr="xlsx_tmp_img_65.png"/>
+        <xdr:cNvPr id="66" name="Picture 65" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -5559,7 +5559,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="67" name="Picture 66" descr="xlsx_tmp_img_66.png"/>
+        <xdr:cNvPr id="67" name="Picture 66" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -5597,7 +5597,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="68" name="Picture 67" descr="xlsx_tmp_img_67.png"/>
+        <xdr:cNvPr id="68" name="Picture 67" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -5635,7 +5635,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="69" name="Picture 68" descr="xlsx_tmp_img_68.png"/>
+        <xdr:cNvPr id="69" name="Picture 68" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -5673,7 +5673,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="70" name="Picture 69" descr="xlsx_tmp_img_69.png"/>
+        <xdr:cNvPr id="70" name="Picture 69" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -5711,7 +5711,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="71" name="Picture 70" descr="xlsx_tmp_img_70.png"/>
+        <xdr:cNvPr id="71" name="Picture 70" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -5749,7 +5749,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="72" name="Picture 71" descr="xlsx_tmp_img_71.png"/>
+        <xdr:cNvPr id="72" name="Picture 71" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -5787,7 +5787,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="73" name="Picture 72" descr="xlsx_tmp_img_72.png"/>
+        <xdr:cNvPr id="73" name="Picture 72" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -5825,7 +5825,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="74" name="Picture 73" descr="xlsx_tmp_img_73.png"/>
+        <xdr:cNvPr id="74" name="Picture 73" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -5863,7 +5863,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="75" name="Picture 74" descr="xlsx_tmp_img_74.png"/>
+        <xdr:cNvPr id="75" name="Picture 74" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -5901,7 +5901,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="76" name="Picture 75" descr="xlsx_tmp_img_75.png"/>
+        <xdr:cNvPr id="76" name="Picture 75" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -5939,7 +5939,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="77" name="Picture 76" descr="xlsx_tmp_img_76.png"/>
+        <xdr:cNvPr id="77" name="Picture 76" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -5977,7 +5977,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="78" name="Picture 77" descr="xlsx_tmp_img_77.png"/>
+        <xdr:cNvPr id="78" name="Picture 77" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -6015,7 +6015,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="79" name="Picture 78" descr="xlsx_tmp_img_78.png"/>
+        <xdr:cNvPr id="79" name="Picture 78" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -6053,7 +6053,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="80" name="Picture 79" descr="xlsx_tmp_img_79.png"/>
+        <xdr:cNvPr id="80" name="Picture 79" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -6091,7 +6091,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="81" name="Picture 80" descr="xlsx_tmp_img_80.png"/>
+        <xdr:cNvPr id="81" name="Picture 80" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -6129,7 +6129,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="82" name="Picture 81" descr="xlsx_tmp_img_81.png"/>
+        <xdr:cNvPr id="82" name="Picture 81" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -6167,7 +6167,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="83" name="Picture 82" descr="xlsx_tmp_img_82.png"/>
+        <xdr:cNvPr id="83" name="Picture 82" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -6205,7 +6205,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="84" name="Picture 83" descr="xlsx_tmp_img_83.png"/>
+        <xdr:cNvPr id="84" name="Picture 83" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -6243,7 +6243,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="85" name="Picture 84" descr="xlsx_tmp_img_84.png"/>
+        <xdr:cNvPr id="85" name="Picture 84" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -6281,7 +6281,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="86" name="Picture 85" descr="xlsx_tmp_img_85.png"/>
+        <xdr:cNvPr id="86" name="Picture 85" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -6319,7 +6319,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="87" name="Picture 86" descr="xlsx_tmp_img_86.png"/>
+        <xdr:cNvPr id="87" name="Picture 86" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -6357,7 +6357,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="88" name="Picture 87" descr="xlsx_tmp_img_87.png"/>
+        <xdr:cNvPr id="88" name="Picture 87" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -6395,7 +6395,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="89" name="Picture 88" descr="xlsx_tmp_img_88.png"/>
+        <xdr:cNvPr id="89" name="Picture 88" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -6433,7 +6433,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="90" name="Picture 89" descr="xlsx_tmp_img_89.png"/>
+        <xdr:cNvPr id="90" name="Picture 89" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -6471,7 +6471,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="91" name="Picture 90" descr="xlsx_tmp_img_90.png"/>
+        <xdr:cNvPr id="91" name="Picture 90" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -6509,7 +6509,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="92" name="Picture 91" descr="xlsx_tmp_img_91.png"/>
+        <xdr:cNvPr id="92" name="Picture 91" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -6547,7 +6547,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="93" name="Picture 92" descr="xlsx_tmp_img_92.png"/>
+        <xdr:cNvPr id="93" name="Picture 92" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -6585,7 +6585,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="94" name="Picture 93" descr="xlsx_tmp_img_93.png"/>
+        <xdr:cNvPr id="94" name="Picture 93" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -6623,7 +6623,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="95" name="Picture 94" descr="xlsx_tmp_img_94.png"/>
+        <xdr:cNvPr id="95" name="Picture 94" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -6661,7 +6661,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="96" name="Picture 95" descr="xlsx_tmp_img_95.png"/>
+        <xdr:cNvPr id="96" name="Picture 95" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -6699,7 +6699,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="97" name="Picture 96" descr="xlsx_tmp_img_96.png"/>
+        <xdr:cNvPr id="97" name="Picture 96" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -6737,7 +6737,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="98" name="Picture 97" descr="xlsx_tmp_img_97.png"/>
+        <xdr:cNvPr id="98" name="Picture 97" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -6775,7 +6775,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="99" name="Picture 98" descr="xlsx_tmp_img_98.png"/>
+        <xdr:cNvPr id="99" name="Picture 98" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -6813,7 +6813,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="100" name="Picture 99" descr="xlsx_tmp_img_99.png"/>
+        <xdr:cNvPr id="100" name="Picture 99" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -6851,7 +6851,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="101" name="Picture 100" descr="xlsx_tmp_img_100.png"/>
+        <xdr:cNvPr id="101" name="Picture 100" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -6889,7 +6889,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="102" name="Picture 101" descr="xlsx_tmp_img_101.png"/>
+        <xdr:cNvPr id="102" name="Picture 101" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -6927,7 +6927,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="103" name="Picture 102" descr="xlsx_tmp_img_102.png"/>
+        <xdr:cNvPr id="103" name="Picture 102" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -6965,7 +6965,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="104" name="Picture 103" descr="xlsx_tmp_img_103.png"/>
+        <xdr:cNvPr id="104" name="Picture 103" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -7003,7 +7003,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="105" name="Picture 104" descr="xlsx_tmp_img_104.png"/>
+        <xdr:cNvPr id="105" name="Picture 104" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -7041,7 +7041,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="106" name="Picture 105" descr="xlsx_tmp_img_105.png"/>
+        <xdr:cNvPr id="106" name="Picture 105" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -7079,7 +7079,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="107" name="Picture 106" descr="xlsx_tmp_img_106.png"/>
+        <xdr:cNvPr id="107" name="Picture 106" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -7117,7 +7117,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="108" name="Picture 107" descr="xlsx_tmp_img_107.png"/>
+        <xdr:cNvPr id="108" name="Picture 107" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -7155,7 +7155,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="109" name="Picture 108" descr="xlsx_tmp_img_108.png"/>
+        <xdr:cNvPr id="109" name="Picture 108" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -7193,7 +7193,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="110" name="Picture 109" descr="xlsx_tmp_img_109.png"/>
+        <xdr:cNvPr id="110" name="Picture 109" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -7231,7 +7231,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="111" name="Picture 110" descr="xlsx_tmp_img_110.png"/>
+        <xdr:cNvPr id="111" name="Picture 110" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -7269,7 +7269,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="112" name="Picture 111" descr="xlsx_tmp_img_111.png"/>
+        <xdr:cNvPr id="112" name="Picture 111" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -7307,7 +7307,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="113" name="Picture 112" descr="xlsx_tmp_img_112.png"/>
+        <xdr:cNvPr id="113" name="Picture 112" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -7345,7 +7345,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="114" name="Picture 113" descr="xlsx_tmp_img_113.png"/>
+        <xdr:cNvPr id="114" name="Picture 113" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -7383,7 +7383,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="115" name="Picture 114" descr="xlsx_tmp_img_114.png"/>
+        <xdr:cNvPr id="115" name="Picture 114" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -7421,7 +7421,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="116" name="Picture 115" descr="xlsx_tmp_img_115.png"/>
+        <xdr:cNvPr id="116" name="Picture 115" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -7459,7 +7459,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="117" name="Picture 116" descr="xlsx_tmp_img_116.png"/>
+        <xdr:cNvPr id="117" name="Picture 116" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -7497,7 +7497,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="118" name="Picture 117" descr="xlsx_tmp_img_117.png"/>
+        <xdr:cNvPr id="118" name="Picture 117" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -7535,7 +7535,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="119" name="Picture 118" descr="xlsx_tmp_img_118.png"/>
+        <xdr:cNvPr id="119" name="Picture 118" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -7573,7 +7573,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="120" name="Picture 119" descr="xlsx_tmp_img_119.png"/>
+        <xdr:cNvPr id="120" name="Picture 119" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -7611,7 +7611,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="121" name="Picture 120" descr="xlsx_tmp_img_120.png"/>
+        <xdr:cNvPr id="121" name="Picture 120" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -7649,7 +7649,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="122" name="Picture 121" descr="xlsx_tmp_img_121.png"/>
+        <xdr:cNvPr id="122" name="Picture 121" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -7687,7 +7687,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="123" name="Picture 122" descr="xlsx_tmp_img_122.png"/>
+        <xdr:cNvPr id="123" name="Picture 122" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -7725,7 +7725,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="124" name="Picture 123" descr="xlsx_tmp_img_123.png"/>
+        <xdr:cNvPr id="124" name="Picture 123" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -7763,7 +7763,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="125" name="Picture 124" descr="xlsx_tmp_img_124.png"/>
+        <xdr:cNvPr id="125" name="Picture 124" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -7801,7 +7801,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="126" name="Picture 125" descr="xlsx_tmp_img_125.png"/>
+        <xdr:cNvPr id="126" name="Picture 125" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -7839,7 +7839,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="127" name="Picture 126" descr="xlsx_tmp_img_126.png"/>
+        <xdr:cNvPr id="127" name="Picture 126" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -7877,7 +7877,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="128" name="Picture 127" descr="xlsx_tmp_img_127.png"/>
+        <xdr:cNvPr id="128" name="Picture 127" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -7915,7 +7915,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="129" name="Picture 128" descr="xlsx_tmp_img_128.png"/>
+        <xdr:cNvPr id="129" name="Picture 128" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -7953,7 +7953,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="130" name="Picture 129" descr="xlsx_tmp_img_129.png"/>
+        <xdr:cNvPr id="130" name="Picture 129" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -7991,7 +7991,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="131" name="Picture 130" descr="xlsx_tmp_img_130.png"/>
+        <xdr:cNvPr id="131" name="Picture 130" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -8029,7 +8029,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="132" name="Picture 131" descr="xlsx_tmp_img_131.png"/>
+        <xdr:cNvPr id="132" name="Picture 131" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -8067,7 +8067,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="133" name="Picture 132" descr="xlsx_tmp_img_132.png"/>
+        <xdr:cNvPr id="133" name="Picture 132" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -8105,7 +8105,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="134" name="Picture 133" descr="xlsx_tmp_img_133.png"/>
+        <xdr:cNvPr id="134" name="Picture 133" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -8143,7 +8143,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="135" name="Picture 134" descr="xlsx_tmp_img_134.png"/>
+        <xdr:cNvPr id="135" name="Picture 134" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -8181,7 +8181,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="136" name="Picture 135" descr="xlsx_tmp_img_135.png"/>
+        <xdr:cNvPr id="136" name="Picture 135" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -8219,7 +8219,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="137" name="Picture 136" descr="xlsx_tmp_img_136.png"/>
+        <xdr:cNvPr id="137" name="Picture 136" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -8257,7 +8257,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="138" name="Picture 137" descr="xlsx_tmp_img_137.png"/>
+        <xdr:cNvPr id="138" name="Picture 137" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -8295,7 +8295,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="139" name="Picture 138" descr="xlsx_tmp_img_138.png"/>
+        <xdr:cNvPr id="139" name="Picture 138" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -8333,7 +8333,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="140" name="Picture 139" descr="xlsx_tmp_img_139.png"/>
+        <xdr:cNvPr id="140" name="Picture 139" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -8371,7 +8371,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="141" name="Picture 140" descr="xlsx_tmp_img_140.png"/>
+        <xdr:cNvPr id="141" name="Picture 140" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -8409,7 +8409,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="142" name="Picture 141" descr="xlsx_tmp_img_141.png"/>
+        <xdr:cNvPr id="142" name="Picture 141" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -8447,7 +8447,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="143" name="Picture 142" descr="xlsx_tmp_img_142.png"/>
+        <xdr:cNvPr id="143" name="Picture 142" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -8485,7 +8485,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="144" name="Picture 143" descr="xlsx_tmp_img_143.png"/>
+        <xdr:cNvPr id="144" name="Picture 143" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -8523,7 +8523,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="145" name="Picture 144" descr="xlsx_tmp_img_144.png"/>
+        <xdr:cNvPr id="145" name="Picture 144" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -8561,7 +8561,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="146" name="Picture 145" descr="xlsx_tmp_img_145.png"/>
+        <xdr:cNvPr id="146" name="Picture 145" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -8599,7 +8599,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="147" name="Picture 146" descr="xlsx_tmp_img_146.png"/>
+        <xdr:cNvPr id="147" name="Picture 146" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -8637,7 +8637,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="148" name="Picture 147" descr="xlsx_tmp_img_147.png"/>
+        <xdr:cNvPr id="148" name="Picture 147" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -8675,7 +8675,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="149" name="Picture 148" descr="xlsx_tmp_img_148.png"/>
+        <xdr:cNvPr id="149" name="Picture 148" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -8713,7 +8713,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="150" name="Picture 149" descr="xlsx_tmp_img_149.png"/>
+        <xdr:cNvPr id="150" name="Picture 149" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -8751,7 +8751,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="151" name="Picture 150" descr="xlsx_tmp_img_150.png"/>
+        <xdr:cNvPr id="151" name="Picture 150" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -8789,7 +8789,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="152" name="Picture 151" descr="xlsx_tmp_img_151.png"/>
+        <xdr:cNvPr id="152" name="Picture 151" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -8827,7 +8827,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="153" name="Picture 152" descr="xlsx_tmp_img_152.png"/>
+        <xdr:cNvPr id="153" name="Picture 152" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -8865,7 +8865,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="154" name="Picture 153" descr="xlsx_tmp_img_153.png"/>
+        <xdr:cNvPr id="154" name="Picture 153" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -8903,7 +8903,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="155" name="Picture 154" descr="xlsx_tmp_img_154.png"/>
+        <xdr:cNvPr id="155" name="Picture 154" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -8941,7 +8941,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="156" name="Picture 155" descr="xlsx_tmp_img_155.png"/>
+        <xdr:cNvPr id="156" name="Picture 155" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -8979,7 +8979,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="157" name="Picture 156" descr="xlsx_tmp_img_156.png"/>
+        <xdr:cNvPr id="157" name="Picture 156" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -9017,7 +9017,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="158" name="Picture 157" descr="xlsx_tmp_img_157.png"/>
+        <xdr:cNvPr id="158" name="Picture 157" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -9055,7 +9055,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="159" name="Picture 158" descr="xlsx_tmp_img_158.png"/>
+        <xdr:cNvPr id="159" name="Picture 158" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -9093,7 +9093,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="160" name="Picture 159" descr="xlsx_tmp_img_159.png"/>
+        <xdr:cNvPr id="160" name="Picture 159" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -9131,7 +9131,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="161" name="Picture 160" descr="xlsx_tmp_img_160.png"/>
+        <xdr:cNvPr id="161" name="Picture 160" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -9169,7 +9169,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="162" name="Picture 161" descr="xlsx_tmp_img_161.png"/>
+        <xdr:cNvPr id="162" name="Picture 161" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -9207,7 +9207,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="163" name="Picture 162" descr="xlsx_tmp_img_162.png"/>
+        <xdr:cNvPr id="163" name="Picture 162" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -9245,7 +9245,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="164" name="Picture 163" descr="xlsx_tmp_img_163.png"/>
+        <xdr:cNvPr id="164" name="Picture 163" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -9283,7 +9283,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="165" name="Picture 164" descr="xlsx_tmp_img_164.png"/>
+        <xdr:cNvPr id="165" name="Picture 164" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -9321,7 +9321,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="166" name="Picture 165" descr="xlsx_tmp_img_165.png"/>
+        <xdr:cNvPr id="166" name="Picture 165" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -9359,7 +9359,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="167" name="Picture 166" descr="xlsx_tmp_img_166.png"/>
+        <xdr:cNvPr id="167" name="Picture 166" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -9397,7 +9397,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="168" name="Picture 167" descr="xlsx_tmp_img_167.png"/>
+        <xdr:cNvPr id="168" name="Picture 167" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -9435,7 +9435,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="169" name="Picture 168" descr="xlsx_tmp_img_168.png"/>
+        <xdr:cNvPr id="169" name="Picture 168" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -9473,7 +9473,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="170" name="Picture 169" descr="xlsx_tmp_img_169.png"/>
+        <xdr:cNvPr id="170" name="Picture 169" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -9511,7 +9511,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="171" name="Picture 170" descr="xlsx_tmp_img_170.png"/>
+        <xdr:cNvPr id="171" name="Picture 170" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -9549,7 +9549,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="172" name="Picture 171" descr="xlsx_tmp_img_171.png"/>
+        <xdr:cNvPr id="172" name="Picture 171" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -9587,7 +9587,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="173" name="Picture 172" descr="xlsx_tmp_img_172.png"/>
+        <xdr:cNvPr id="173" name="Picture 172" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -9625,7 +9625,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="174" name="Picture 173" descr="xlsx_tmp_img_173.png"/>
+        <xdr:cNvPr id="174" name="Picture 173" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -9663,7 +9663,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="175" name="Picture 174" descr="xlsx_tmp_img_174.png"/>
+        <xdr:cNvPr id="175" name="Picture 174" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -9701,7 +9701,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="176" name="Picture 175" descr="xlsx_tmp_img_175.png"/>
+        <xdr:cNvPr id="176" name="Picture 175" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -9739,7 +9739,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="177" name="Picture 176" descr="xlsx_tmp_img_176.png"/>
+        <xdr:cNvPr id="177" name="Picture 176" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -9777,7 +9777,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="178" name="Picture 177" descr="xlsx_tmp_img_177.png"/>
+        <xdr:cNvPr id="178" name="Picture 177" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -9815,7 +9815,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="179" name="Picture 178" descr="xlsx_tmp_img_178.png"/>
+        <xdr:cNvPr id="179" name="Picture 178" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -9853,7 +9853,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="180" name="Picture 179" descr="xlsx_tmp_img_179.png"/>
+        <xdr:cNvPr id="180" name="Picture 179" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -9891,7 +9891,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="181" name="Picture 180" descr="xlsx_tmp_img_180.png"/>
+        <xdr:cNvPr id="181" name="Picture 180" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -9929,7 +9929,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="182" name="Picture 181" descr="xlsx_tmp_img_181.png"/>
+        <xdr:cNvPr id="182" name="Picture 181" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -9967,7 +9967,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="183" name="Picture 182" descr="xlsx_tmp_img_182.png"/>
+        <xdr:cNvPr id="183" name="Picture 182" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -10005,7 +10005,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="184" name="Picture 183" descr="xlsx_tmp_img_183.png"/>
+        <xdr:cNvPr id="184" name="Picture 183" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -10043,7 +10043,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="185" name="Picture 184" descr="xlsx_tmp_img_184.png"/>
+        <xdr:cNvPr id="185" name="Picture 184" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -10081,7 +10081,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="186" name="Picture 185" descr="xlsx_tmp_img_185.png"/>
+        <xdr:cNvPr id="186" name="Picture 185" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -10119,7 +10119,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="187" name="Picture 186" descr="xlsx_tmp_img_186.png"/>
+        <xdr:cNvPr id="187" name="Picture 186" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -10157,7 +10157,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="188" name="Picture 187" descr="xlsx_tmp_img_187.png"/>
+        <xdr:cNvPr id="188" name="Picture 187" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -10195,7 +10195,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="189" name="Picture 188" descr="xlsx_tmp_img_188.png"/>
+        <xdr:cNvPr id="189" name="Picture 188" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -10233,7 +10233,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="190" name="Picture 189" descr="xlsx_tmp_img_189.png"/>
+        <xdr:cNvPr id="190" name="Picture 189" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -10271,7 +10271,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="191" name="Picture 190" descr="xlsx_tmp_img_190.png"/>
+        <xdr:cNvPr id="191" name="Picture 190" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -10309,7 +10309,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="192" name="Picture 191" descr="xlsx_tmp_img_191.png"/>
+        <xdr:cNvPr id="192" name="Picture 191" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -10347,7 +10347,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="193" name="Picture 192" descr="xlsx_tmp_img_192.png"/>
+        <xdr:cNvPr id="193" name="Picture 192" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -10385,7 +10385,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="194" name="Picture 193" descr="xlsx_tmp_img_193.png"/>
+        <xdr:cNvPr id="194" name="Picture 193" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -10423,7 +10423,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="195" name="Picture 194" descr="xlsx_tmp_img_194.png"/>
+        <xdr:cNvPr id="195" name="Picture 194" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -10461,7 +10461,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="196" name="Picture 195" descr="xlsx_tmp_img_195.png"/>
+        <xdr:cNvPr id="196" name="Picture 195" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -10499,7 +10499,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="197" name="Picture 196" descr="xlsx_tmp_img_196.png"/>
+        <xdr:cNvPr id="197" name="Picture 196" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -10537,7 +10537,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="198" name="Picture 197" descr="xlsx_tmp_img_197.png"/>
+        <xdr:cNvPr id="198" name="Picture 197" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -10575,7 +10575,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="199" name="Picture 198" descr="xlsx_tmp_img_198.png"/>
+        <xdr:cNvPr id="199" name="Picture 198" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -10613,7 +10613,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="200" name="Picture 199" descr="xlsx_tmp_img_199.png"/>
+        <xdr:cNvPr id="200" name="Picture 199" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -10651,7 +10651,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="201" name="Picture 200" descr="xlsx_tmp_img_200.png"/>
+        <xdr:cNvPr id="201" name="Picture 200" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -10689,7 +10689,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="202" name="Picture 201" descr="xlsx_tmp_img_201.png"/>
+        <xdr:cNvPr id="202" name="Picture 201" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -10727,7 +10727,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="203" name="Picture 202" descr="xlsx_tmp_img_202.png"/>
+        <xdr:cNvPr id="203" name="Picture 202" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -10765,7 +10765,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="204" name="Picture 203" descr="xlsx_tmp_img_203.png"/>
+        <xdr:cNvPr id="204" name="Picture 203" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -10803,7 +10803,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="205" name="Picture 204" descr="xlsx_tmp_img_204.png"/>
+        <xdr:cNvPr id="205" name="Picture 204" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -10841,7 +10841,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="206" name="Picture 205" descr="xlsx_tmp_img_205.png"/>
+        <xdr:cNvPr id="206" name="Picture 205" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -10879,7 +10879,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="207" name="Picture 206" descr="xlsx_tmp_img_206.png"/>
+        <xdr:cNvPr id="207" name="Picture 206" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -10917,7 +10917,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="208" name="Picture 207" descr="xlsx_tmp_img_207.png"/>
+        <xdr:cNvPr id="208" name="Picture 207" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -10955,7 +10955,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="209" name="Picture 208" descr="xlsx_tmp_img_208.png"/>
+        <xdr:cNvPr id="209" name="Picture 208" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -10993,7 +10993,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="210" name="Picture 209" descr="xlsx_tmp_img_209.png"/>
+        <xdr:cNvPr id="210" name="Picture 209" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -11031,7 +11031,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="211" name="Picture 210" descr="xlsx_tmp_img_210.png"/>
+        <xdr:cNvPr id="211" name="Picture 210" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -11069,7 +11069,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="212" name="Picture 211" descr="xlsx_tmp_img_211.png"/>
+        <xdr:cNvPr id="212" name="Picture 211" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -11107,7 +11107,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="213" name="Picture 212" descr="xlsx_tmp_img_212.png"/>
+        <xdr:cNvPr id="213" name="Picture 212" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -11145,7 +11145,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="214" name="Picture 213" descr="xlsx_tmp_img_213.png"/>
+        <xdr:cNvPr id="214" name="Picture 213" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -11183,7 +11183,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="215" name="Picture 214" descr="xlsx_tmp_img_214.png"/>
+        <xdr:cNvPr id="215" name="Picture 214" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -11221,7 +11221,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="216" name="Picture 215" descr="xlsx_tmp_img_215.png"/>
+        <xdr:cNvPr id="216" name="Picture 215" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -11259,7 +11259,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="217" name="Picture 216" descr="xlsx_tmp_img_216.png"/>
+        <xdr:cNvPr id="217" name="Picture 216" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -11297,7 +11297,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="218" name="Picture 217" descr="xlsx_tmp_img_217.png"/>
+        <xdr:cNvPr id="218" name="Picture 217" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -11335,7 +11335,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="219" name="Picture 218" descr="xlsx_tmp_img_218.png"/>
+        <xdr:cNvPr id="219" name="Picture 218" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -11373,7 +11373,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="220" name="Picture 219" descr="xlsx_tmp_img_219.png"/>
+        <xdr:cNvPr id="220" name="Picture 219" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -11411,7 +11411,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="221" name="Picture 220" descr="xlsx_tmp_img_220.png"/>
+        <xdr:cNvPr id="221" name="Picture 220" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -11449,7 +11449,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="222" name="Picture 221" descr="xlsx_tmp_img_221.png"/>
+        <xdr:cNvPr id="222" name="Picture 221" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -11487,7 +11487,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="223" name="Picture 222" descr="xlsx_tmp_img_222.png"/>
+        <xdr:cNvPr id="223" name="Picture 222" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -11525,7 +11525,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="224" name="Picture 223" descr="xlsx_tmp_img_223.png"/>
+        <xdr:cNvPr id="224" name="Picture 223" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -11563,7 +11563,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="225" name="Picture 224" descr="xlsx_tmp_img_224.png"/>
+        <xdr:cNvPr id="225" name="Picture 224" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -11601,7 +11601,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="226" name="Picture 225" descr="xlsx_tmp_img_225.png"/>
+        <xdr:cNvPr id="226" name="Picture 225" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -11639,7 +11639,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="227" name="Picture 226" descr="xlsx_tmp_img_226.png"/>
+        <xdr:cNvPr id="227" name="Picture 226" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -11677,7 +11677,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="228" name="Picture 227" descr="xlsx_tmp_img_227.png"/>
+        <xdr:cNvPr id="228" name="Picture 227" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -11715,7 +11715,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="229" name="Picture 228" descr="xlsx_tmp_img_228.png"/>
+        <xdr:cNvPr id="229" name="Picture 228" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -11753,7 +11753,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="230" name="Picture 229" descr="xlsx_tmp_img_229.png"/>
+        <xdr:cNvPr id="230" name="Picture 229" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -11791,7 +11791,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="231" name="Picture 230" descr="xlsx_tmp_img_230.png"/>
+        <xdr:cNvPr id="231" name="Picture 230" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -11829,7 +11829,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="232" name="Picture 231" descr="xlsx_tmp_img_231.png"/>
+        <xdr:cNvPr id="232" name="Picture 231" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -11867,7 +11867,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="233" name="Picture 232" descr="xlsx_tmp_img_232.png"/>
+        <xdr:cNvPr id="233" name="Picture 232" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -11905,7 +11905,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="234" name="Picture 233" descr="xlsx_tmp_img_233.png"/>
+        <xdr:cNvPr id="234" name="Picture 233" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -11943,7 +11943,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="235" name="Picture 234" descr="xlsx_tmp_img_234.png"/>
+        <xdr:cNvPr id="235" name="Picture 234" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -11981,7 +11981,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="236" name="Picture 235" descr="xlsx_tmp_img_235.png"/>
+        <xdr:cNvPr id="236" name="Picture 235" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -12019,7 +12019,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="237" name="Picture 236" descr="xlsx_tmp_img_236.png"/>
+        <xdr:cNvPr id="237" name="Picture 236" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -12057,7 +12057,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="238" name="Picture 237" descr="xlsx_tmp_img_237.png"/>
+        <xdr:cNvPr id="238" name="Picture 237" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -12095,7 +12095,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="239" name="Picture 238" descr="xlsx_tmp_img_238.png"/>
+        <xdr:cNvPr id="239" name="Picture 238" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -12133,7 +12133,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="240" name="Picture 239" descr="xlsx_tmp_img_239.png"/>
+        <xdr:cNvPr id="240" name="Picture 239" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -12171,7 +12171,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="241" name="Picture 240" descr="xlsx_tmp_img_240.png"/>
+        <xdr:cNvPr id="241" name="Picture 240" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -12209,7 +12209,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="242" name="Picture 241" descr="xlsx_tmp_img_241.png"/>
+        <xdr:cNvPr id="242" name="Picture 241" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -12247,7 +12247,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="243" name="Picture 242" descr="xlsx_tmp_img_242.png"/>
+        <xdr:cNvPr id="243" name="Picture 242" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -12285,7 +12285,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="244" name="Picture 243" descr="xlsx_tmp_img_243.png"/>
+        <xdr:cNvPr id="244" name="Picture 243" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -12323,7 +12323,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="245" name="Picture 244" descr="xlsx_tmp_img_244.png"/>
+        <xdr:cNvPr id="245" name="Picture 244" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -12361,7 +12361,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="246" name="Picture 245" descr="xlsx_tmp_img_245.png"/>
+        <xdr:cNvPr id="246" name="Picture 245" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -12399,7 +12399,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="247" name="Picture 246" descr="xlsx_tmp_img_246.png"/>
+        <xdr:cNvPr id="247" name="Picture 246" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -12437,7 +12437,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="248" name="Picture 247" descr="xlsx_tmp_img_247.png"/>
+        <xdr:cNvPr id="248" name="Picture 247" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -12475,7 +12475,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="249" name="Picture 248" descr="xlsx_tmp_img_248.png"/>
+        <xdr:cNvPr id="249" name="Picture 248" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -12513,7 +12513,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="250" name="Picture 249" descr="xlsx_tmp_img_249.png"/>
+        <xdr:cNvPr id="250" name="Picture 249" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -12551,7 +12551,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="251" name="Picture 250" descr="xlsx_tmp_img_250.png"/>
+        <xdr:cNvPr id="251" name="Picture 250" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -12589,7 +12589,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="252" name="Picture 251" descr="xlsx_tmp_img_251.png"/>
+        <xdr:cNvPr id="252" name="Picture 251" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -12627,7 +12627,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="253" name="Picture 252" descr="xlsx_tmp_img_252.png"/>
+        <xdr:cNvPr id="253" name="Picture 252" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -12665,7 +12665,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="254" name="Picture 253" descr="xlsx_tmp_img_253.png"/>
+        <xdr:cNvPr id="254" name="Picture 253" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -12703,7 +12703,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="255" name="Picture 254" descr="xlsx_tmp_img_254.png"/>
+        <xdr:cNvPr id="255" name="Picture 254" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -12741,7 +12741,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="256" name="Picture 255" descr="xlsx_tmp_img_255.png"/>
+        <xdr:cNvPr id="256" name="Picture 255" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -12779,7 +12779,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="257" name="Picture 256" descr="xlsx_tmp_img_256.png"/>
+        <xdr:cNvPr id="257" name="Picture 256" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -12817,7 +12817,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="258" name="Picture 257" descr="xlsx_tmp_img_257.png"/>
+        <xdr:cNvPr id="258" name="Picture 257" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -12855,7 +12855,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="259" name="Picture 258" descr="xlsx_tmp_img_258.png"/>
+        <xdr:cNvPr id="259" name="Picture 258" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -12893,7 +12893,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="260" name="Picture 259" descr="xlsx_tmp_img_259.png"/>
+        <xdr:cNvPr id="260" name="Picture 259" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -12931,7 +12931,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="261" name="Picture 260" descr="xlsx_tmp_img_260.png"/>
+        <xdr:cNvPr id="261" name="Picture 260" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -12969,7 +12969,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="262" name="Picture 261" descr="xlsx_tmp_img_261.png"/>
+        <xdr:cNvPr id="262" name="Picture 261" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -13007,7 +13007,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="263" name="Picture 262" descr="xlsx_tmp_img_262.png"/>
+        <xdr:cNvPr id="263" name="Picture 262" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -13045,7 +13045,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="264" name="Picture 263" descr="xlsx_tmp_img_263.png"/>
+        <xdr:cNvPr id="264" name="Picture 263" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -13083,7 +13083,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="265" name="Picture 264" descr="xlsx_tmp_img_264.png"/>
+        <xdr:cNvPr id="265" name="Picture 264" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -13121,7 +13121,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="266" name="Picture 265" descr="xlsx_tmp_img_265.png"/>
+        <xdr:cNvPr id="266" name="Picture 265" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -13159,7 +13159,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="267" name="Picture 266" descr="xlsx_tmp_img_266.png"/>
+        <xdr:cNvPr id="267" name="Picture 266" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -13197,7 +13197,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="268" name="Picture 267" descr="xlsx_tmp_img_267.png"/>
+        <xdr:cNvPr id="268" name="Picture 267" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -13235,7 +13235,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="269" name="Picture 268" descr="xlsx_tmp_img_268.png"/>
+        <xdr:cNvPr id="269" name="Picture 268" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -13273,7 +13273,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="270" name="Picture 269" descr="xlsx_tmp_img_269.png"/>
+        <xdr:cNvPr id="270" name="Picture 269" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -13311,7 +13311,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="271" name="Picture 270" descr="xlsx_tmp_img_270.png"/>
+        <xdr:cNvPr id="271" name="Picture 270" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -13349,7 +13349,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="272" name="Picture 271" descr="xlsx_tmp_img_271.png"/>
+        <xdr:cNvPr id="272" name="Picture 271" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -13387,7 +13387,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="273" name="Picture 272" descr="xlsx_tmp_img_272.png"/>
+        <xdr:cNvPr id="273" name="Picture 272" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -13425,7 +13425,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="274" name="Picture 273" descr="xlsx_tmp_img_273.png"/>
+        <xdr:cNvPr id="274" name="Picture 273" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -13463,7 +13463,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="275" name="Picture 274" descr="xlsx_tmp_img_274.png"/>
+        <xdr:cNvPr id="275" name="Picture 274" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -13501,7 +13501,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="276" name="Picture 275" descr="xlsx_tmp_img_275.png"/>
+        <xdr:cNvPr id="276" name="Picture 275" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -13539,7 +13539,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="277" name="Picture 276" descr="xlsx_tmp_img_276.png"/>
+        <xdr:cNvPr id="277" name="Picture 276" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -13577,7 +13577,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="278" name="Picture 277" descr="xlsx_tmp_img_277.png"/>
+        <xdr:cNvPr id="278" name="Picture 277" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -13615,7 +13615,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="279" name="Picture 278" descr="xlsx_tmp_img_278.png"/>
+        <xdr:cNvPr id="279" name="Picture 278" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -13653,7 +13653,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="280" name="Picture 279" descr="xlsx_tmp_img_279.png"/>
+        <xdr:cNvPr id="280" name="Picture 279" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -13691,7 +13691,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="281" name="Picture 280" descr="xlsx_tmp_img_280.png"/>
+        <xdr:cNvPr id="281" name="Picture 280" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -13729,7 +13729,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="282" name="Picture 281" descr="xlsx_tmp_img_281.png"/>
+        <xdr:cNvPr id="282" name="Picture 281" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -13767,7 +13767,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="283" name="Picture 282" descr="xlsx_tmp_img_282.png"/>
+        <xdr:cNvPr id="283" name="Picture 282" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -13805,7 +13805,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="284" name="Picture 283" descr="xlsx_tmp_img_283.png"/>
+        <xdr:cNvPr id="284" name="Picture 283" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -13843,7 +13843,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="285" name="Picture 284" descr="xlsx_tmp_img_284.png"/>
+        <xdr:cNvPr id="285" name="Picture 284" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -13881,7 +13881,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="286" name="Picture 285" descr="xlsx_tmp_img_285.png"/>
+        <xdr:cNvPr id="286" name="Picture 285" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -13919,7 +13919,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="287" name="Picture 286" descr="xlsx_tmp_img_286.png"/>
+        <xdr:cNvPr id="287" name="Picture 286" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -13957,7 +13957,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="288" name="Picture 287" descr="xlsx_tmp_img_287.png"/>
+        <xdr:cNvPr id="288" name="Picture 287" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -13995,7 +13995,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="289" name="Picture 288" descr="xlsx_tmp_img_288.png"/>
+        <xdr:cNvPr id="289" name="Picture 288" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -14033,7 +14033,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="290" name="Picture 289" descr="xlsx_tmp_img_289.png"/>
+        <xdr:cNvPr id="290" name="Picture 289" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -14071,7 +14071,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="291" name="Picture 290" descr="xlsx_tmp_img_290.png"/>
+        <xdr:cNvPr id="291" name="Picture 290" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -14109,7 +14109,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="292" name="Picture 291" descr="xlsx_tmp_img_291.png"/>
+        <xdr:cNvPr id="292" name="Picture 291" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -14147,7 +14147,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="293" name="Picture 292" descr="xlsx_tmp_img_292.png"/>
+        <xdr:cNvPr id="293" name="Picture 292" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -14185,7 +14185,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="294" name="Picture 293" descr="xlsx_tmp_img_293.png"/>
+        <xdr:cNvPr id="294" name="Picture 293" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -14223,7 +14223,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="295" name="Picture 294" descr="xlsx_tmp_img_294.png"/>
+        <xdr:cNvPr id="295" name="Picture 294" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -14261,7 +14261,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="296" name="Picture 295" descr="xlsx_tmp_img_295.png"/>
+        <xdr:cNvPr id="296" name="Picture 295" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -14299,7 +14299,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="297" name="Picture 296" descr="xlsx_tmp_img_296.png"/>
+        <xdr:cNvPr id="297" name="Picture 296" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -14337,7 +14337,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="298" name="Picture 297" descr="xlsx_tmp_img_297.png"/>
+        <xdr:cNvPr id="298" name="Picture 297" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -14375,7 +14375,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="299" name="Picture 298" descr="xlsx_tmp_img_298.png"/>
+        <xdr:cNvPr id="299" name="Picture 298" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -14413,7 +14413,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="300" name="Picture 299" descr="xlsx_tmp_img_299.png"/>
+        <xdr:cNvPr id="300" name="Picture 299" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -14451,7 +14451,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="301" name="Picture 300" descr="xlsx_tmp_img_300.png"/>
+        <xdr:cNvPr id="301" name="Picture 300" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -14489,7 +14489,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="302" name="Picture 301" descr="xlsx_tmp_img_301.png"/>
+        <xdr:cNvPr id="302" name="Picture 301" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -14527,7 +14527,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="303" name="Picture 302" descr="xlsx_tmp_img_302.png"/>
+        <xdr:cNvPr id="303" name="Picture 302" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -14565,7 +14565,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="304" name="Picture 303" descr="xlsx_tmp_img_303.png"/>
+        <xdr:cNvPr id="304" name="Picture 303" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -14603,7 +14603,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="305" name="Picture 304" descr="xlsx_tmp_img_304.png"/>
+        <xdr:cNvPr id="305" name="Picture 304" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -14641,7 +14641,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="306" name="Picture 305" descr="xlsx_tmp_img_305.png"/>
+        <xdr:cNvPr id="306" name="Picture 305" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -14679,7 +14679,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="307" name="Picture 306" descr="xlsx_tmp_img_306.png"/>
+        <xdr:cNvPr id="307" name="Picture 306" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -14717,7 +14717,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="308" name="Picture 307" descr="xlsx_tmp_img_307.png"/>
+        <xdr:cNvPr id="308" name="Picture 307" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -14755,7 +14755,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="309" name="Picture 308" descr="xlsx_tmp_img_308.png"/>
+        <xdr:cNvPr id="309" name="Picture 308" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -14793,7 +14793,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="310" name="Picture 309" descr="xlsx_tmp_img_309.png"/>
+        <xdr:cNvPr id="310" name="Picture 309" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -14831,7 +14831,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="311" name="Picture 310" descr="xlsx_tmp_img_310.png"/>
+        <xdr:cNvPr id="311" name="Picture 310" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -14869,7 +14869,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="312" name="Picture 311" descr="xlsx_tmp_img_311.png"/>
+        <xdr:cNvPr id="312" name="Picture 311" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -14907,7 +14907,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="313" name="Picture 312" descr="xlsx_tmp_img_312.png"/>
+        <xdr:cNvPr id="313" name="Picture 312" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -14945,7 +14945,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="314" name="Picture 313" descr="xlsx_tmp_img_313.png"/>
+        <xdr:cNvPr id="314" name="Picture 313" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -14983,7 +14983,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="315" name="Picture 314" descr="xlsx_tmp_img_314.png"/>
+        <xdr:cNvPr id="315" name="Picture 314" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -15021,7 +15021,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="316" name="Picture 315" descr="xlsx_tmp_img_315.png"/>
+        <xdr:cNvPr id="316" name="Picture 315" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -15059,7 +15059,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="317" name="Picture 316" descr="xlsx_tmp_img_316.png"/>
+        <xdr:cNvPr id="317" name="Picture 316" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -15097,7 +15097,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="318" name="Picture 317" descr="xlsx_tmp_img_317.png"/>
+        <xdr:cNvPr id="318" name="Picture 317" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -15135,7 +15135,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="319" name="Picture 318" descr="xlsx_tmp_img_318.png"/>
+        <xdr:cNvPr id="319" name="Picture 318" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -15173,7 +15173,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="320" name="Picture 319" descr="xlsx_tmp_img_319.png"/>
+        <xdr:cNvPr id="320" name="Picture 319" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -15211,7 +15211,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="321" name="Picture 320" descr="xlsx_tmp_img_320.png"/>
+        <xdr:cNvPr id="321" name="Picture 320" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -15249,7 +15249,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="322" name="Picture 321" descr="xlsx_tmp_img_321.png"/>
+        <xdr:cNvPr id="322" name="Picture 321" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -15287,7 +15287,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="323" name="Picture 322" descr="xlsx_tmp_img_322.png"/>
+        <xdr:cNvPr id="323" name="Picture 322" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -15325,7 +15325,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="324" name="Picture 323" descr="xlsx_tmp_img_323.png"/>
+        <xdr:cNvPr id="324" name="Picture 323" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -15363,7 +15363,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="325" name="Picture 324" descr="xlsx_tmp_img_324.png"/>
+        <xdr:cNvPr id="325" name="Picture 324" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -15401,7 +15401,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="326" name="Picture 325" descr="xlsx_tmp_img_325.png"/>
+        <xdr:cNvPr id="326" name="Picture 325" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -15439,7 +15439,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="327" name="Picture 326" descr="xlsx_tmp_img_326.png"/>
+        <xdr:cNvPr id="327" name="Picture 326" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -15477,7 +15477,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="328" name="Picture 327" descr="xlsx_tmp_img_327.png"/>
+        <xdr:cNvPr id="328" name="Picture 327" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -15515,7 +15515,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="329" name="Picture 328" descr="xlsx_tmp_img_328.png"/>
+        <xdr:cNvPr id="329" name="Picture 328" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -15553,7 +15553,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="330" name="Picture 329" descr="xlsx_tmp_img_329.png"/>
+        <xdr:cNvPr id="330" name="Picture 329" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -15591,7 +15591,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="331" name="Picture 330" descr="xlsx_tmp_img_330.png"/>
+        <xdr:cNvPr id="331" name="Picture 330" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -15629,7 +15629,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="332" name="Picture 331" descr="xlsx_tmp_img_331.png"/>
+        <xdr:cNvPr id="332" name="Picture 331" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -15667,7 +15667,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="333" name="Picture 332" descr="xlsx_tmp_img_332.png"/>
+        <xdr:cNvPr id="333" name="Picture 332" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -15705,7 +15705,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="334" name="Picture 333" descr="xlsx_tmp_img_333.png"/>
+        <xdr:cNvPr id="334" name="Picture 333" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -15743,7 +15743,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="335" name="Picture 334" descr="xlsx_tmp_img_334.png"/>
+        <xdr:cNvPr id="335" name="Picture 334" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -15781,7 +15781,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="336" name="Picture 335" descr="xlsx_tmp_img_335.png"/>
+        <xdr:cNvPr id="336" name="Picture 335" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -15819,7 +15819,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="337" name="Picture 336" descr="xlsx_tmp_img_336.png"/>
+        <xdr:cNvPr id="337" name="Picture 336" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -15857,7 +15857,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="338" name="Picture 337" descr="xlsx_tmp_img_337.png"/>
+        <xdr:cNvPr id="338" name="Picture 337" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -15895,7 +15895,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="339" name="Picture 338" descr="xlsx_tmp_img_338.png"/>
+        <xdr:cNvPr id="339" name="Picture 338" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -15933,7 +15933,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="340" name="Picture 339" descr="xlsx_tmp_img_339.png"/>
+        <xdr:cNvPr id="340" name="Picture 339" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -15971,7 +15971,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="341" name="Picture 340" descr="xlsx_tmp_img_340.png"/>
+        <xdr:cNvPr id="341" name="Picture 340" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -16009,7 +16009,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="342" name="Picture 341" descr="xlsx_tmp_img_341.png"/>
+        <xdr:cNvPr id="342" name="Picture 341" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -16047,7 +16047,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="343" name="Picture 342" descr="xlsx_tmp_img_342.png"/>
+        <xdr:cNvPr id="343" name="Picture 342" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -16085,7 +16085,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="344" name="Picture 343" descr="xlsx_tmp_img_343.png"/>
+        <xdr:cNvPr id="344" name="Picture 343" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -16123,7 +16123,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="345" name="Picture 344" descr="xlsx_tmp_img_344.png"/>
+        <xdr:cNvPr id="345" name="Picture 344" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -16161,7 +16161,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="346" name="Picture 345" descr="xlsx_tmp_img_345.png"/>
+        <xdr:cNvPr id="346" name="Picture 345" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -16199,7 +16199,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="347" name="Picture 346" descr="xlsx_tmp_img_346.png"/>
+        <xdr:cNvPr id="347" name="Picture 346" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -16237,7 +16237,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="348" name="Picture 347" descr="xlsx_tmp_img_347.png"/>
+        <xdr:cNvPr id="348" name="Picture 347" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -16275,7 +16275,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="349" name="Picture 348" descr="xlsx_tmp_img_348.png"/>
+        <xdr:cNvPr id="349" name="Picture 348" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -16313,7 +16313,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="350" name="Picture 349" descr="xlsx_tmp_img_349.png"/>
+        <xdr:cNvPr id="350" name="Picture 349" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -16351,7 +16351,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="351" name="Picture 350" descr="xlsx_tmp_img_350.png"/>
+        <xdr:cNvPr id="351" name="Picture 350" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -16389,7 +16389,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="352" name="Picture 351" descr="xlsx_tmp_img_351.png"/>
+        <xdr:cNvPr id="352" name="Picture 351" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -16427,7 +16427,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="353" name="Picture 352" descr="xlsx_tmp_img_352.png"/>
+        <xdr:cNvPr id="353" name="Picture 352" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -16465,7 +16465,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="354" name="Picture 353" descr="xlsx_tmp_img_353.png"/>
+        <xdr:cNvPr id="354" name="Picture 353" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -16503,7 +16503,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="355" name="Picture 354" descr="xlsx_tmp_img_354.png"/>
+        <xdr:cNvPr id="355" name="Picture 354" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -16541,7 +16541,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="356" name="Picture 355" descr="xlsx_tmp_img_355.png"/>
+        <xdr:cNvPr id="356" name="Picture 355" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -16579,7 +16579,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="357" name="Picture 356" descr="xlsx_tmp_img_356.png"/>
+        <xdr:cNvPr id="357" name="Picture 356" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -16617,7 +16617,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="358" name="Picture 357" descr="xlsx_tmp_img_357.png"/>
+        <xdr:cNvPr id="358" name="Picture 357" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -16655,7 +16655,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="359" name="Picture 358" descr="xlsx_tmp_img_358.png"/>
+        <xdr:cNvPr id="359" name="Picture 358" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -16693,7 +16693,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="360" name="Picture 359" descr="xlsx_tmp_img_359.png"/>
+        <xdr:cNvPr id="360" name="Picture 359" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -16731,7 +16731,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="361" name="Picture 360" descr="xlsx_tmp_img_360.png"/>
+        <xdr:cNvPr id="361" name="Picture 360" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -16769,7 +16769,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="362" name="Picture 361" descr="xlsx_tmp_img_361.png"/>
+        <xdr:cNvPr id="362" name="Picture 361" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -16807,7 +16807,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="363" name="Picture 362" descr="xlsx_tmp_img_362.png"/>
+        <xdr:cNvPr id="363" name="Picture 362" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -16845,7 +16845,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="364" name="Picture 363" descr="xlsx_tmp_img_363.png"/>
+        <xdr:cNvPr id="364" name="Picture 363" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -16883,7 +16883,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="365" name="Picture 364" descr="xlsx_tmp_img_364.png"/>
+        <xdr:cNvPr id="365" name="Picture 364" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -16921,7 +16921,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="366" name="Picture 365" descr="xlsx_tmp_img_365.png"/>
+        <xdr:cNvPr id="366" name="Picture 365" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -16959,7 +16959,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="367" name="Picture 366" descr="xlsx_tmp_img_366.png"/>
+        <xdr:cNvPr id="367" name="Picture 366" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -16997,7 +16997,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="368" name="Picture 367" descr="xlsx_tmp_img_367.png"/>
+        <xdr:cNvPr id="368" name="Picture 367" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -17035,7 +17035,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="369" name="Picture 368" descr="xlsx_tmp_img_368.png"/>
+        <xdr:cNvPr id="369" name="Picture 368" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -17073,7 +17073,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="370" name="Picture 369" descr="xlsx_tmp_img_369.png"/>
+        <xdr:cNvPr id="370" name="Picture 369" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -17111,7 +17111,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="371" name="Picture 370" descr="xlsx_tmp_img_370.png"/>
+        <xdr:cNvPr id="371" name="Picture 370" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -17149,7 +17149,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="372" name="Picture 371" descr="xlsx_tmp_img_371.png"/>
+        <xdr:cNvPr id="372" name="Picture 371" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -17187,7 +17187,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="373" name="Picture 372" descr="xlsx_tmp_img_372.png"/>
+        <xdr:cNvPr id="373" name="Picture 372" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -17225,7 +17225,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="374" name="Picture 373" descr="xlsx_tmp_img_373.png"/>
+        <xdr:cNvPr id="374" name="Picture 373" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -17263,7 +17263,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="375" name="Picture 374" descr="xlsx_tmp_img_374.png"/>
+        <xdr:cNvPr id="375" name="Picture 374" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -17301,7 +17301,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="376" name="Picture 375" descr="xlsx_tmp_img_375.png"/>
+        <xdr:cNvPr id="376" name="Picture 375" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -17339,7 +17339,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="377" name="Picture 376" descr="xlsx_tmp_img_376.png"/>
+        <xdr:cNvPr id="377" name="Picture 376" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -17377,7 +17377,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="378" name="Picture 377" descr="xlsx_tmp_img_377.png"/>
+        <xdr:cNvPr id="378" name="Picture 377" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -17415,7 +17415,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="379" name="Picture 378" descr="xlsx_tmp_img_378.png"/>
+        <xdr:cNvPr id="379" name="Picture 378" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -17453,7 +17453,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="380" name="Picture 379" descr="xlsx_tmp_img_379.png"/>
+        <xdr:cNvPr id="380" name="Picture 379" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -17491,7 +17491,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="381" name="Picture 380" descr="xlsx_tmp_img_380.png"/>
+        <xdr:cNvPr id="381" name="Picture 380" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -17529,7 +17529,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="382" name="Picture 381" descr="xlsx_tmp_img_381.png"/>
+        <xdr:cNvPr id="382" name="Picture 381" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -17567,7 +17567,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="383" name="Picture 382" descr="xlsx_tmp_img_382.png"/>
+        <xdr:cNvPr id="383" name="Picture 382" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -17605,7 +17605,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="384" name="Picture 383" descr="xlsx_tmp_img_383.png"/>
+        <xdr:cNvPr id="384" name="Picture 383" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -17643,7 +17643,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="385" name="Picture 384" descr="xlsx_tmp_img_384.png"/>
+        <xdr:cNvPr id="385" name="Picture 384" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -17681,7 +17681,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="386" name="Picture 385" descr="xlsx_tmp_img_385.png"/>
+        <xdr:cNvPr id="386" name="Picture 385" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -17719,7 +17719,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="387" name="Picture 386" descr="xlsx_tmp_img_386.png"/>
+        <xdr:cNvPr id="387" name="Picture 386" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -17757,7 +17757,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="388" name="Picture 387" descr="xlsx_tmp_img_387.png"/>
+        <xdr:cNvPr id="388" name="Picture 387" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -17795,7 +17795,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="389" name="Picture 388" descr="xlsx_tmp_img_388.png"/>
+        <xdr:cNvPr id="389" name="Picture 388" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -17833,7 +17833,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="390" name="Picture 389" descr="xlsx_tmp_img_389.png"/>
+        <xdr:cNvPr id="390" name="Picture 389" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -17871,7 +17871,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="391" name="Picture 390" descr="xlsx_tmp_img_390.png"/>
+        <xdr:cNvPr id="391" name="Picture 390" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -17909,7 +17909,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="392" name="Picture 391" descr="xlsx_tmp_img_391.png"/>
+        <xdr:cNvPr id="392" name="Picture 391" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -17947,7 +17947,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="393" name="Picture 392" descr="xlsx_tmp_img_392.png"/>
+        <xdr:cNvPr id="393" name="Picture 392" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -17985,7 +17985,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="394" name="Picture 393" descr="xlsx_tmp_img_393.png"/>
+        <xdr:cNvPr id="394" name="Picture 393" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -18023,7 +18023,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="395" name="Picture 394" descr="xlsx_tmp_img_394.png"/>
+        <xdr:cNvPr id="395" name="Picture 394" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -18061,7 +18061,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="396" name="Picture 395" descr="xlsx_tmp_img_395.png"/>
+        <xdr:cNvPr id="396" name="Picture 395" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -18099,7 +18099,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="397" name="Picture 396" descr="xlsx_tmp_img_396.png"/>
+        <xdr:cNvPr id="397" name="Picture 396" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -18137,7 +18137,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="398" name="Picture 397" descr="xlsx_tmp_img_397.png"/>
+        <xdr:cNvPr id="398" name="Picture 397" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -18175,7 +18175,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="399" name="Picture 398" descr="xlsx_tmp_img_398.png"/>
+        <xdr:cNvPr id="399" name="Picture 398" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -18213,7 +18213,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="400" name="Picture 399" descr="xlsx_tmp_img_399.png"/>
+        <xdr:cNvPr id="400" name="Picture 399" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -18251,7 +18251,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="401" name="Picture 400" descr="xlsx_tmp_img_400.png"/>
+        <xdr:cNvPr id="401" name="Picture 400" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -18289,7 +18289,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="402" name="Picture 401" descr="xlsx_tmp_img_401.png"/>
+        <xdr:cNvPr id="402" name="Picture 401" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -18327,7 +18327,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="403" name="Picture 402" descr="xlsx_tmp_img_402.png"/>
+        <xdr:cNvPr id="403" name="Picture 402" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -18365,7 +18365,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="404" name="Picture 403" descr="xlsx_tmp_img_403.png"/>
+        <xdr:cNvPr id="404" name="Picture 403" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -18403,7 +18403,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="405" name="Picture 404" descr="xlsx_tmp_img_404.png"/>
+        <xdr:cNvPr id="405" name="Picture 404" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -18441,7 +18441,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="406" name="Picture 405" descr="xlsx_tmp_img_405.png"/>
+        <xdr:cNvPr id="406" name="Picture 405" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -18479,7 +18479,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="407" name="Picture 406" descr="xlsx_tmp_img_406.png"/>
+        <xdr:cNvPr id="407" name="Picture 406" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -18517,7 +18517,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="408" name="Picture 407" descr="xlsx_tmp_img_407.png"/>
+        <xdr:cNvPr id="408" name="Picture 407" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -18555,7 +18555,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="409" name="Picture 408" descr="xlsx_tmp_img_408.png"/>
+        <xdr:cNvPr id="409" name="Picture 408" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -18593,7 +18593,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="410" name="Picture 409" descr="xlsx_tmp_img_409.png"/>
+        <xdr:cNvPr id="410" name="Picture 409" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -18631,7 +18631,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="411" name="Picture 410" descr="xlsx_tmp_img_410.png"/>
+        <xdr:cNvPr id="411" name="Picture 410" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -18669,7 +18669,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="412" name="Picture 411" descr="xlsx_tmp_img_411.png"/>
+        <xdr:cNvPr id="412" name="Picture 411" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -18707,7 +18707,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="413" name="Picture 412" descr="xlsx_tmp_img_412.png"/>
+        <xdr:cNvPr id="413" name="Picture 412" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -18745,7 +18745,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="414" name="Picture 413" descr="xlsx_tmp_img_413.png"/>
+        <xdr:cNvPr id="414" name="Picture 413" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -18783,7 +18783,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="415" name="Picture 414" descr="xlsx_tmp_img_414.png"/>
+        <xdr:cNvPr id="415" name="Picture 414" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -18821,7 +18821,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="416" name="Picture 415" descr="xlsx_tmp_img_415.png"/>
+        <xdr:cNvPr id="416" name="Picture 415" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -18859,7 +18859,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="417" name="Picture 416" descr="xlsx_tmp_img_416.png"/>
+        <xdr:cNvPr id="417" name="Picture 416" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -18897,7 +18897,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="418" name="Picture 417" descr="xlsx_tmp_img_417.png"/>
+        <xdr:cNvPr id="418" name="Picture 417" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -18935,7 +18935,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="419" name="Picture 418" descr="xlsx_tmp_img_418.png"/>
+        <xdr:cNvPr id="419" name="Picture 418" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -18973,7 +18973,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="420" name="Picture 419" descr="xlsx_tmp_img_419.png"/>
+        <xdr:cNvPr id="420" name="Picture 419" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -19011,7 +19011,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="421" name="Picture 420" descr="xlsx_tmp_img_420.png"/>
+        <xdr:cNvPr id="421" name="Picture 420" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -19049,7 +19049,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="422" name="Picture 421" descr="xlsx_tmp_img_421.png"/>
+        <xdr:cNvPr id="422" name="Picture 421" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -19087,7 +19087,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="423" name="Picture 422" descr="xlsx_tmp_img_422.png"/>
+        <xdr:cNvPr id="423" name="Picture 422" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -19125,7 +19125,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="424" name="Picture 423" descr="xlsx_tmp_img_423.png"/>
+        <xdr:cNvPr id="424" name="Picture 423" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -19163,7 +19163,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="425" name="Picture 424" descr="xlsx_tmp_img_424.png"/>
+        <xdr:cNvPr id="425" name="Picture 424" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -19201,7 +19201,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="426" name="Picture 425" descr="xlsx_tmp_img_425.png"/>
+        <xdr:cNvPr id="426" name="Picture 425" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -19239,7 +19239,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="427" name="Picture 426" descr="xlsx_tmp_img_426.png"/>
+        <xdr:cNvPr id="427" name="Picture 426" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -19277,7 +19277,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="428" name="Picture 427" descr="xlsx_tmp_img_427.png"/>
+        <xdr:cNvPr id="428" name="Picture 427" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -19315,7 +19315,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="429" name="Picture 428" descr="xlsx_tmp_img_428.png"/>
+        <xdr:cNvPr id="429" name="Picture 428" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -19353,7 +19353,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="430" name="Picture 429" descr="xlsx_tmp_img_429.png"/>
+        <xdr:cNvPr id="430" name="Picture 429" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -19391,7 +19391,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="431" name="Picture 430" descr="xlsx_tmp_img_430.png"/>
+        <xdr:cNvPr id="431" name="Picture 430" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -19429,7 +19429,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="432" name="Picture 431" descr="xlsx_tmp_img_431.png"/>
+        <xdr:cNvPr id="432" name="Picture 431" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -19467,7 +19467,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="433" name="Picture 432" descr="xlsx_tmp_img_432.png"/>
+        <xdr:cNvPr id="433" name="Picture 432" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -19505,7 +19505,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="434" name="Picture 433" descr="xlsx_tmp_img_433.png"/>
+        <xdr:cNvPr id="434" name="Picture 433" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -19543,7 +19543,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="435" name="Picture 434" descr="xlsx_tmp_img_434.png"/>
+        <xdr:cNvPr id="435" name="Picture 434" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -19581,7 +19581,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="436" name="Picture 435" descr="xlsx_tmp_img_435.png"/>
+        <xdr:cNvPr id="436" name="Picture 435" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -19619,7 +19619,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="437" name="Picture 436" descr="xlsx_tmp_img_436.png"/>
+        <xdr:cNvPr id="437" name="Picture 436" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -19657,7 +19657,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="438" name="Picture 437" descr="xlsx_tmp_img_437.png"/>
+        <xdr:cNvPr id="438" name="Picture 437" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -19695,7 +19695,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="439" name="Picture 438" descr="xlsx_tmp_img_438.png"/>
+        <xdr:cNvPr id="439" name="Picture 438" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -19733,7 +19733,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="440" name="Picture 439" descr="xlsx_tmp_img_439.png"/>
+        <xdr:cNvPr id="440" name="Picture 439" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -19771,7 +19771,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="441" name="Picture 440" descr="xlsx_tmp_img_440.png"/>
+        <xdr:cNvPr id="441" name="Picture 440" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -19809,7 +19809,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="442" name="Picture 441" descr="xlsx_tmp_img_441.png"/>
+        <xdr:cNvPr id="442" name="Picture 441" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -19847,7 +19847,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="443" name="Picture 442" descr="xlsx_tmp_img_442.png"/>
+        <xdr:cNvPr id="443" name="Picture 442" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -19885,7 +19885,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="444" name="Picture 443" descr="xlsx_tmp_img_443.png"/>
+        <xdr:cNvPr id="444" name="Picture 443" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -19923,7 +19923,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="445" name="Picture 444" descr="xlsx_tmp_img_444.png"/>
+        <xdr:cNvPr id="445" name="Picture 444" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -19961,7 +19961,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="446" name="Picture 445" descr="xlsx_tmp_img_445.png"/>
+        <xdr:cNvPr id="446" name="Picture 445" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -19999,7 +19999,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="447" name="Picture 446" descr="xlsx_tmp_img_446.png"/>
+        <xdr:cNvPr id="447" name="Picture 446" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -20037,7 +20037,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="448" name="Picture 447" descr="xlsx_tmp_img_447.png"/>
+        <xdr:cNvPr id="448" name="Picture 447" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -20075,7 +20075,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="449" name="Picture 448" descr="xlsx_tmp_img_448.png"/>
+        <xdr:cNvPr id="449" name="Picture 448" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -20113,7 +20113,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="450" name="Picture 449" descr="xlsx_tmp_img_449.png"/>
+        <xdr:cNvPr id="450" name="Picture 449" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -20151,7 +20151,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="451" name="Picture 450" descr="xlsx_tmp_img_450.png"/>
+        <xdr:cNvPr id="451" name="Picture 450" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -20189,7 +20189,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="452" name="Picture 451" descr="xlsx_tmp_img_451.png"/>
+        <xdr:cNvPr id="452" name="Picture 451" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -20227,7 +20227,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="453" name="Picture 452" descr="xlsx_tmp_img_452.png"/>
+        <xdr:cNvPr id="453" name="Picture 452" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -20265,7 +20265,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="454" name="Picture 453" descr="xlsx_tmp_img_453.png"/>
+        <xdr:cNvPr id="454" name="Picture 453" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -20303,7 +20303,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="455" name="Picture 454" descr="xlsx_tmp_img_454.png"/>
+        <xdr:cNvPr id="455" name="Picture 454" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -20341,7 +20341,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="456" name="Picture 455" descr="xlsx_tmp_img_455.png"/>
+        <xdr:cNvPr id="456" name="Picture 455" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -20379,7 +20379,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="457" name="Picture 456" descr="xlsx_tmp_img_456.png"/>
+        <xdr:cNvPr id="457" name="Picture 456" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -20417,7 +20417,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="458" name="Picture 457" descr="xlsx_tmp_img_457.png"/>
+        <xdr:cNvPr id="458" name="Picture 457" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -20455,7 +20455,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="459" name="Picture 458" descr="xlsx_tmp_img_458.png"/>
+        <xdr:cNvPr id="459" name="Picture 458" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -20493,7 +20493,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="460" name="Picture 459" descr="xlsx_tmp_img_459.png"/>
+        <xdr:cNvPr id="460" name="Picture 459" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -20531,7 +20531,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="461" name="Picture 460" descr="xlsx_tmp_img_460.png"/>
+        <xdr:cNvPr id="461" name="Picture 460" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -20569,7 +20569,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="462" name="Picture 461" descr="xlsx_tmp_img_461.png"/>
+        <xdr:cNvPr id="462" name="Picture 461" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -20607,7 +20607,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="463" name="Picture 462" descr="xlsx_tmp_img_462.png"/>
+        <xdr:cNvPr id="463" name="Picture 462" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -20645,7 +20645,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="464" name="Picture 463" descr="xlsx_tmp_img_463.png"/>
+        <xdr:cNvPr id="464" name="Picture 463" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -20683,7 +20683,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="465" name="Picture 464" descr="xlsx_tmp_img_464.png"/>
+        <xdr:cNvPr id="465" name="Picture 464" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -20721,7 +20721,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="466" name="Picture 465" descr="xlsx_tmp_img_465.png"/>
+        <xdr:cNvPr id="466" name="Picture 465" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -20759,7 +20759,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="467" name="Picture 466" descr="xlsx_tmp_img_466.png"/>
+        <xdr:cNvPr id="467" name="Picture 466" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -20797,7 +20797,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="468" name="Picture 467" descr="xlsx_tmp_img_467.png"/>
+        <xdr:cNvPr id="468" name="Picture 467" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -20835,7 +20835,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="469" name="Picture 468" descr="xlsx_tmp_img_468.png"/>
+        <xdr:cNvPr id="469" name="Picture 468" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -20873,7 +20873,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="470" name="Picture 469" descr="xlsx_tmp_img_469.png"/>
+        <xdr:cNvPr id="470" name="Picture 469" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -20911,7 +20911,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="471" name="Picture 470" descr="xlsx_tmp_img_470.png"/>
+        <xdr:cNvPr id="471" name="Picture 470" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -20949,7 +20949,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="472" name="Picture 471" descr="xlsx_tmp_img_471.png"/>
+        <xdr:cNvPr id="472" name="Picture 471" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -20987,7 +20987,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="473" name="Picture 472" descr="xlsx_tmp_img_472.png"/>
+        <xdr:cNvPr id="473" name="Picture 472" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -21025,7 +21025,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="474" name="Picture 473" descr="xlsx_tmp_img_473.png"/>
+        <xdr:cNvPr id="474" name="Picture 473" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -21063,7 +21063,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="475" name="Picture 474" descr="xlsx_tmp_img_474.png"/>
+        <xdr:cNvPr id="475" name="Picture 474" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -21101,7 +21101,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="476" name="Picture 475" descr="xlsx_tmp_img_475.png"/>
+        <xdr:cNvPr id="476" name="Picture 475" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -21139,7 +21139,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="477" name="Picture 476" descr="xlsx_tmp_img_476.png"/>
+        <xdr:cNvPr id="477" name="Picture 476" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -21177,7 +21177,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="478" name="Picture 477" descr="xlsx_tmp_img_477.png"/>
+        <xdr:cNvPr id="478" name="Picture 477" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -21215,7 +21215,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="479" name="Picture 478" descr="xlsx_tmp_img_478.png"/>
+        <xdr:cNvPr id="479" name="Picture 478" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -21253,7 +21253,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="480" name="Picture 479" descr="xlsx_tmp_img_479.png"/>
+        <xdr:cNvPr id="480" name="Picture 479" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -21291,7 +21291,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="481" name="Picture 480" descr="xlsx_tmp_img_480.png"/>
+        <xdr:cNvPr id="481" name="Picture 480" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -21329,7 +21329,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="482" name="Picture 481" descr="xlsx_tmp_img_481.png"/>
+        <xdr:cNvPr id="482" name="Picture 481" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -21367,7 +21367,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="483" name="Picture 482" descr="xlsx_tmp_img_482.png"/>
+        <xdr:cNvPr id="483" name="Picture 482" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -21405,7 +21405,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="484" name="Picture 483" descr="xlsx_tmp_img_483.png"/>
+        <xdr:cNvPr id="484" name="Picture 483" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -21443,7 +21443,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="485" name="Picture 484" descr="xlsx_tmp_img_484.png"/>
+        <xdr:cNvPr id="485" name="Picture 484" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -21481,7 +21481,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="486" name="Picture 485" descr="xlsx_tmp_img_485.png"/>
+        <xdr:cNvPr id="486" name="Picture 485" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -21519,7 +21519,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="487" name="Picture 486" descr="xlsx_tmp_img_486.png"/>
+        <xdr:cNvPr id="487" name="Picture 486" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -21557,7 +21557,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="488" name="Picture 487" descr="xlsx_tmp_img_487.png"/>
+        <xdr:cNvPr id="488" name="Picture 487" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -21595,7 +21595,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="489" name="Picture 488" descr="xlsx_tmp_img_488.png"/>
+        <xdr:cNvPr id="489" name="Picture 488" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -21633,7 +21633,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="490" name="Picture 489" descr="xlsx_tmp_img_489.png"/>
+        <xdr:cNvPr id="490" name="Picture 489" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -21671,7 +21671,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="491" name="Picture 490" descr="xlsx_tmp_img_490.png"/>
+        <xdr:cNvPr id="491" name="Picture 490" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -21709,7 +21709,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="492" name="Picture 491" descr="xlsx_tmp_img_491.png"/>
+        <xdr:cNvPr id="492" name="Picture 491" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -21747,7 +21747,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="493" name="Picture 492" descr="xlsx_tmp_img_492.png"/>
+        <xdr:cNvPr id="493" name="Picture 492" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -21785,7 +21785,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="494" name="Picture 493" descr="xlsx_tmp_img_493.png"/>
+        <xdr:cNvPr id="494" name="Picture 493" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -21823,7 +21823,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="495" name="Picture 494" descr="xlsx_tmp_img_494.png"/>
+        <xdr:cNvPr id="495" name="Picture 494" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -21861,7 +21861,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="496" name="Picture 495" descr="xlsx_tmp_img_495.png"/>
+        <xdr:cNvPr id="496" name="Picture 495" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -21899,7 +21899,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="497" name="Picture 496" descr="xlsx_tmp_img_496.png"/>
+        <xdr:cNvPr id="497" name="Picture 496" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -21937,7 +21937,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="498" name="Picture 497" descr="xlsx_tmp_img_497.png"/>
+        <xdr:cNvPr id="498" name="Picture 497" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -21975,7 +21975,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="499" name="Picture 498" descr="xlsx_tmp_img_498.png"/>
+        <xdr:cNvPr id="499" name="Picture 498" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -22013,7 +22013,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="500" name="Picture 499" descr="xlsx_tmp_img_499.png"/>
+        <xdr:cNvPr id="500" name="Picture 499" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -22051,7 +22051,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="501" name="Picture 500" descr="xlsx_tmp_img_500.png"/>
+        <xdr:cNvPr id="501" name="Picture 500" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>

</xml_diff>